<commit_message>
Updates for labels etc
</commit_message>
<xml_diff>
--- a/BAFDR_M_analysis.xlsx
+++ b/BAFDR_M_analysis.xlsx
@@ -8,20 +8,77 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\JWD\Calculators\Tools\BAFDR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B86B134-4AE4-4575-909F-A10447DBE11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8C893F65-7F29-4064-A238-3F37E53ACEED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19080" yWindow="-120" windowWidth="29040" windowHeight="16440"/>
   </bookViews>
   <sheets>
-    <sheet name="BAFDR-M-output" sheetId="1" r:id="rId1"/>
-    <sheet name="Inputs" sheetId="2" r:id="rId2"/>
+    <sheet name="BAFDR_M_ouputs" sheetId="2" r:id="rId1"/>
+    <sheet name="BAFDR_M_inputs" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+  <si>
+    <t>atomos_mtnum</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> emittance</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wvl1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> wvl2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> focal_lenght</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Diameter_of_aperture</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> pixel_pitch</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> transmission_of_lens</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DWL1_detector_cuton</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DWL2_detector_cutoff</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ScaleFactor_for_DarkCurrent</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> QE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OperTemp_Detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vn_Amp_Ampin_ROIC_Amp_noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Vmax_ROIC_Voltage</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Res_ADC_ROIC_Bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CifF_Integration_Capacitor</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tint_Integration_time</t>
+  </si>
   <si>
     <t xml:space="preserve"> Radiance</t>
   </si>
@@ -89,7 +146,7 @@
     <t>SHOT</t>
   </si>
   <si>
-    <t>Tint</t>
+    <t xml:space="preserve"> Tint</t>
   </si>
 </sst>
 </file>
@@ -621,75 +678,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -741,6 +737,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NETD vs Tint</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -781,7 +802,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'BAFDR-M-output'!$V$1</c:f>
+              <c:f>BAFDR_M_ouputs!$X$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -816,9 +837,9 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'BAFDR-M-output'!$U$2:$U$16</c:f>
+              <c:f>BAFDR_M_ouputs!$W$2:$W$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>9.9999999999999995E-8</c:v>
@@ -870,7 +891,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'BAFDR-M-output'!$V$2:$V$16</c:f>
+              <c:f>BAFDR_M_ouputs!$X$2:$X$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -925,7 +946,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3E12-477E-B7B8-F6E150C41BC9}"/>
+              <c16:uniqueId val="{00000000-A9A0-4F51-B401-FFEE19767906}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -937,13 +958,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1139184495"/>
-        <c:axId val="1254853104"/>
+        <c:axId val="93911503"/>
+        <c:axId val="94783279"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1139184495"/>
+        <c:axId val="93911503"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1.0000000000000002E-2"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -962,6 +985,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Integration Time (sec)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -991,7 +1039,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1028,16 +1076,16 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1254853104"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="94783279"/>
+        <c:crossesAt val="1.0000000000000002E-2"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1254853104"/>
+        <c:axId val="94783279"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
-          <c:max val="10"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1056,6 +1104,31 @@
           </c:spPr>
         </c:majorGridlines>
         <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>NETD (K)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1122,7 +1195,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1139184495"/>
+        <c:crossAx val="93911503"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1134,37 +1207,6 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1769,23 +1811,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>581024</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3F2CFA0-A5DD-862D-7F05-E45AB1BBF895}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22977651-CCE5-FD4B-170D-F569ABF2636F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2103,80 +2145,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V16"/>
+  <dimension ref="A1:X16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y28" sqref="Y28"/>
+      <selection activeCell="V33" sqref="V33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="U1" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" t="s">
-        <v>19</v>
+        <v>37</v>
+      </c>
+      <c r="T1" t="s">
+        <v>38</v>
+      </c>
+      <c r="W1" t="s">
+        <v>41</v>
+      </c>
+      <c r="X1" t="s">
+        <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2596701118475820</v>
       </c>
@@ -2211,7 +2256,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="M2">
         <v>69.75</v>
@@ -2234,14 +2279,17 @@
       <c r="S2" s="1">
         <v>3.5396495424739498E-10</v>
       </c>
-      <c r="U2">
+      <c r="T2">
+        <v>183.78422693704999</v>
+      </c>
+      <c r="W2" s="1">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>183.78422693704999</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2596701118475820</v>
       </c>
@@ -2276,7 +2324,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="M3">
         <v>69.75</v>
@@ -2299,14 +2347,17 @@
       <c r="S3" s="1">
         <v>3.5481576525024797E-11</v>
       </c>
-      <c r="U3">
+      <c r="T3">
+        <v>18.4225981524764</v>
+      </c>
+      <c r="W3" s="1">
         <v>9.9999999999999995E-7</v>
       </c>
-      <c r="V3">
+      <c r="X3">
         <v>18.4225981524764</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2596701118475820</v>
       </c>
@@ -2341,7 +2392,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L4" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="M4">
         <v>69.75</v>
@@ -2364,14 +2415,17 @@
       <c r="S4" s="1">
         <v>7.96809437266408E-13</v>
       </c>
-      <c r="U4">
+      <c r="T4">
+        <v>0.41371611705321998</v>
+      </c>
+      <c r="W4" s="1">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>0.41371611705321998</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2596701118475820</v>
       </c>
@@ -2406,7 +2460,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="M5">
         <v>69.75</v>
@@ -2429,14 +2483,17 @@
       <c r="S5" s="1">
         <v>4.3843865602108199E-13</v>
       </c>
-      <c r="U5">
+      <c r="T5">
+        <v>0.227644314752798</v>
+      </c>
+      <c r="W5" s="1">
         <v>1E-4</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>0.227644314752798</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2596701118475820</v>
       </c>
@@ -2471,7 +2528,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L6" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M6">
         <v>69.75</v>
@@ -2494,14 +2551,17 @@
       <c r="S6" s="1">
         <v>1.3568279731911999E-13</v>
       </c>
-      <c r="U6">
+      <c r="T6">
+        <v>7.0448663673416498E-2</v>
+      </c>
+      <c r="W6" s="1">
         <v>5.0000000000000001E-4</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>7.0448663673416498E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2596701118475820</v>
       </c>
@@ -2536,7 +2596,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L7" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M7">
         <v>69.75</v>
@@ -2559,14 +2619,17 @@
       <c r="S7" s="1">
         <v>8.9177737684482795E-14</v>
       </c>
-      <c r="U7">
+      <c r="T7">
+        <v>4.6302497983692202E-2</v>
+      </c>
+      <c r="W7" s="1">
         <v>1E-3</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>4.6302497983692202E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2596701118475820</v>
       </c>
@@ -2601,7 +2664,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L8" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M8">
         <v>69.75</v>
@@ -2624,14 +2687,17 @@
       <c r="S8" s="1">
         <v>6.0524986475414701E-14</v>
       </c>
-      <c r="U8">
+      <c r="T8">
+        <v>3.1425534410350099E-2</v>
+      </c>
+      <c r="W8" s="1">
         <v>2E-3</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>3.1425534410350099E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2596701118475820</v>
       </c>
@@ -2666,7 +2732,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L9" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M9">
         <v>69.75</v>
@@ -2689,14 +2755,17 @@
       <c r="S9" s="1">
         <v>4.87094823123915E-14</v>
       </c>
-      <c r="U9">
+      <c r="T9">
+        <v>2.5290736961009901E-2</v>
+      </c>
+      <c r="W9" s="1">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>2.5290736961009901E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2596701118475820</v>
       </c>
@@ -2731,7 +2800,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L10" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M10">
         <v>69.75</v>
@@ -2754,14 +2823,17 @@
       <c r="S10" s="1">
         <v>4.1873283589557998E-14</v>
       </c>
-      <c r="U10">
+      <c r="T10">
+        <v>2.1741273991899498E-2</v>
+      </c>
+      <c r="W10" s="1">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>2.1741273991899498E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2596701118475820</v>
       </c>
@@ -2796,7 +2868,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L11" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M11">
         <v>69.75</v>
@@ -2819,14 +2891,17 @@
       <c r="S11" s="1">
         <v>3.7285051755371803E-14</v>
       </c>
-      <c r="U11">
+      <c r="T11">
+        <v>1.9358991140065201E-2</v>
+      </c>
+      <c r="W11" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>1.9358991140065201E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2596701118475820</v>
       </c>
@@ -2861,7 +2936,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M12">
         <v>69.75</v>
@@ -2884,14 +2959,17 @@
       <c r="S12" s="1">
         <v>3.3934088139482002E-14</v>
       </c>
-      <c r="U12">
+      <c r="T12">
+        <v>1.7619117601030999E-2</v>
+      </c>
+      <c r="W12" s="1">
         <v>6.0000000000000001E-3</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>1.7619117601030999E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2596701118475820</v>
       </c>
@@ -2926,7 +3004,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L13" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M13">
         <v>69.75</v>
@@ -2949,14 +3027,17 @@
       <c r="S13" s="1">
         <v>3.1349000314682103E-14</v>
       </c>
-      <c r="U13">
+      <c r="T13">
+        <v>1.6276898938577901E-2</v>
+      </c>
+      <c r="W13" s="1">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="V13">
+      <c r="X13">
         <v>1.6276898938577901E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2596701118475820</v>
       </c>
@@ -2991,7 +3072,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L14" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M14">
         <v>69.75</v>
@@ -3014,14 +3095,17 @@
       <c r="S14" s="1">
         <v>2.9276606026783798E-14</v>
       </c>
-      <c r="U14">
+      <c r="T14">
+        <v>1.5200878904560801E-2</v>
+      </c>
+      <c r="W14" s="1">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="V14">
+      <c r="X14">
         <v>1.5200878904560801E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2596701118475820</v>
       </c>
@@ -3056,7 +3140,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M15">
         <v>69.75</v>
@@ -3079,14 +3163,17 @@
       <c r="S15" s="1">
         <v>2.7567220945100501E-14</v>
       </c>
-      <c r="U15">
+      <c r="T15">
+        <v>1.43133390167692E-2</v>
+      </c>
+      <c r="W15" s="1">
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <v>1.43133390167692E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2596701118475820</v>
       </c>
@@ -3121,7 +3208,7 @@
         <v>572.31220386721805</v>
       </c>
       <c r="L16" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="M16">
         <v>69.75</v>
@@ -3144,30 +3231,23 @@
       <c r="S16" s="1">
         <v>2.6125947327205E-14</v>
       </c>
-      <c r="U16">
+      <c r="T16">
+        <v>1.3565006859895401E-2</v>
+      </c>
+      <c r="W16" s="1">
         <v>0.01</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <v>1.3565006859895401E-2</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="J14:J16">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="J2:J16">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J1">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
-      <formula>100</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
-      <formula>"SHOT"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L1:L16">
+  <conditionalFormatting sqref="L2:L16">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"SHOT"</formula>
     </cfRule>
@@ -3179,71 +3259,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S15"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:S15"/>
+      <selection activeCell="S1" sqref="S1:S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>2</v>
-      </c>
-      <c r="B1">
-        <v>0.9</v>
-      </c>
-      <c r="C1">
-        <v>300</v>
-      </c>
-      <c r="D1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="F1">
-        <v>0.4</v>
-      </c>
-      <c r="G1">
-        <v>0.2</v>
-      </c>
-      <c r="H1">
-        <v>20</v>
-      </c>
-      <c r="I1">
-        <v>0.85</v>
-      </c>
-      <c r="J1">
-        <v>2</v>
-      </c>
-      <c r="K1">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="L1">
-        <v>1</v>
-      </c>
-      <c r="M1">
-        <v>0.8</v>
-      </c>
-      <c r="N1">
-        <v>120</v>
-      </c>
-      <c r="O1">
-        <v>1E-4</v>
-      </c>
-      <c r="P1">
-        <v>2</v>
-      </c>
-      <c r="Q1">
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
         <v>14</v>
       </c>
-      <c r="R1">
-        <v>8000</v>
-      </c>
-      <c r="S1">
-        <v>9.9999999999999995E-8</v>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -3289,7 +3369,7 @@
       <c r="N2">
         <v>120</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <v>1E-4</v>
       </c>
       <c r="P2">
@@ -3301,8 +3381,8 @@
       <c r="R2">
         <v>8000</v>
       </c>
-      <c r="S2">
-        <v>9.9999999999999995E-7</v>
+      <c r="S2" s="1">
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -3348,7 +3428,7 @@
       <c r="N3">
         <v>120</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <v>1E-4</v>
       </c>
       <c r="P3">
@@ -3360,8 +3440,8 @@
       <c r="R3">
         <v>8000</v>
       </c>
-      <c r="S3">
-        <v>5.0000000000000002E-5</v>
+      <c r="S3" s="1">
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -3407,7 +3487,7 @@
       <c r="N4">
         <v>120</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="1">
         <v>1E-4</v>
       </c>
       <c r="P4">
@@ -3419,8 +3499,8 @@
       <c r="R4">
         <v>8000</v>
       </c>
-      <c r="S4">
-        <v>1E-4</v>
+      <c r="S4" s="1">
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -3466,7 +3546,7 @@
       <c r="N5">
         <v>120</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <v>1E-4</v>
       </c>
       <c r="P5">
@@ -3478,8 +3558,8 @@
       <c r="R5">
         <v>8000</v>
       </c>
-      <c r="S5">
-        <v>5.0000000000000001E-4</v>
+      <c r="S5" s="1">
+        <v>1E-4</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -3525,7 +3605,7 @@
       <c r="N6">
         <v>120</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <v>1E-4</v>
       </c>
       <c r="P6">
@@ -3537,8 +3617,8 @@
       <c r="R6">
         <v>8000</v>
       </c>
-      <c r="S6">
-        <v>1E-3</v>
+      <c r="S6" s="1">
+        <v>5.0000000000000001E-4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -3584,7 +3664,7 @@
       <c r="N7">
         <v>120</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="1">
         <v>1E-4</v>
       </c>
       <c r="P7">
@@ -3596,8 +3676,8 @@
       <c r="R7">
         <v>8000</v>
       </c>
-      <c r="S7">
-        <v>2E-3</v>
+      <c r="S7" s="1">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -3643,7 +3723,7 @@
       <c r="N8">
         <v>120</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
         <v>1E-4</v>
       </c>
       <c r="P8">
@@ -3655,8 +3735,8 @@
       <c r="R8">
         <v>8000</v>
       </c>
-      <c r="S8">
-        <v>3.0000000000000001E-3</v>
+      <c r="S8" s="1">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -3702,7 +3782,7 @@
       <c r="N9">
         <v>120</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="1">
         <v>1E-4</v>
       </c>
       <c r="P9">
@@ -3714,8 +3794,8 @@
       <c r="R9">
         <v>8000</v>
       </c>
-      <c r="S9">
-        <v>4.0000000000000001E-3</v>
+      <c r="S9" s="1">
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -3761,7 +3841,7 @@
       <c r="N10">
         <v>120</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="1">
         <v>1E-4</v>
       </c>
       <c r="P10">
@@ -3773,8 +3853,8 @@
       <c r="R10">
         <v>8000</v>
       </c>
-      <c r="S10">
-        <v>5.0000000000000001E-3</v>
+      <c r="S10" s="1">
+        <v>4.0000000000000001E-3</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -3820,7 +3900,7 @@
       <c r="N11">
         <v>120</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
         <v>1E-4</v>
       </c>
       <c r="P11">
@@ -3832,8 +3912,8 @@
       <c r="R11">
         <v>8000</v>
       </c>
-      <c r="S11">
-        <v>6.0000000000000001E-3</v>
+      <c r="S11" s="1">
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -3879,7 +3959,7 @@
       <c r="N12">
         <v>120</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="1">
         <v>1E-4</v>
       </c>
       <c r="P12">
@@ -3891,8 +3971,8 @@
       <c r="R12">
         <v>8000</v>
       </c>
-      <c r="S12">
-        <v>7.0000000000000001E-3</v>
+      <c r="S12" s="1">
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -3938,7 +4018,7 @@
       <c r="N13">
         <v>120</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="1">
         <v>1E-4</v>
       </c>
       <c r="P13">
@@ -3950,8 +4030,8 @@
       <c r="R13">
         <v>8000</v>
       </c>
-      <c r="S13">
-        <v>8.0000000000000002E-3</v>
+      <c r="S13" s="1">
+        <v>7.0000000000000001E-3</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -3997,7 +4077,7 @@
       <c r="N14">
         <v>120</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="1">
         <v>1E-4</v>
       </c>
       <c r="P14">
@@ -4009,8 +4089,8 @@
       <c r="R14">
         <v>8000</v>
       </c>
-      <c r="S14">
-        <v>8.9999999999999993E-3</v>
+      <c r="S14" s="1">
+        <v>8.0000000000000002E-3</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -4056,7 +4136,7 @@
       <c r="N15">
         <v>120</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="1">
         <v>1E-4</v>
       </c>
       <c r="P15">
@@ -4068,7 +4148,66 @@
       <c r="R15">
         <v>8000</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="1">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>0.9</v>
+      </c>
+      <c r="C16">
+        <v>300</v>
+      </c>
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <v>5</v>
+      </c>
+      <c r="F16">
+        <v>0.4</v>
+      </c>
+      <c r="G16">
+        <v>0.2</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+      <c r="I16">
+        <v>0.85</v>
+      </c>
+      <c r="J16">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+      <c r="M16">
+        <v>0.8</v>
+      </c>
+      <c r="N16">
+        <v>120</v>
+      </c>
+      <c r="O16" s="1">
+        <v>1E-4</v>
+      </c>
+      <c r="P16">
+        <v>2</v>
+      </c>
+      <c r="Q16">
+        <v>14</v>
+      </c>
+      <c r="R16">
+        <v>8000</v>
+      </c>
+      <c r="S16" s="1">
         <v>0.01</v>
       </c>
     </row>

</xml_diff>